<commit_message>
static complete for shopping
</commit_message>
<xml_diff>
--- a/Findings/Findings.xlsx
+++ b/Findings/Findings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GIT\TLS-pinning-analysis-android\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GIT\TLS-pinning-analysis-android\Findings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDA98218-0027-418E-9087-F1DD8A206D6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AD81DD8-BD45-46D2-B780-DFBA1331F429}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1668" yWindow="504" windowWidth="21000" windowHeight="11232" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="পত্রক1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
   <si>
     <t>1 is found</t>
   </si>
@@ -276,6 +276,24 @@
   </si>
   <si>
     <t>has 2 end cert, has CertificatePinner.smali, cleartext traffic permitted for domain</t>
+  </si>
+  <si>
+    <t>has CertificatePinner.smali, has 2 cert file including root, default network security config,</t>
+  </si>
+  <si>
+    <t>using only http</t>
+  </si>
+  <si>
+    <t>has CertificatePinner.smali, has 10 sha256 on networking/l.smali same file containing of okhttp, cleartext not permitted for dimains except system</t>
+  </si>
+  <si>
+    <t>has CertificatePinner.smali and CertificatePinner.kt</t>
+  </si>
+  <si>
+    <t>has 2 cert file includiing root, has "Certificate pinning failure!" string, default security config, has all possible TLS handshake combination as string</t>
+  </si>
+  <si>
+    <t>defalt cecurity config, has string "Certificate pinning failure!", has cert factory and 9 end cert</t>
   </si>
 </sst>
 </file>
@@ -338,14 +356,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -566,8 +583,8 @@
   </sheetPr>
   <dimension ref="B1:G52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -743,7 +760,7 @@
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="6" t="s">
+      <c r="B25" t="s">
         <v>25</v>
       </c>
       <c r="C25">
@@ -779,48 +796,84 @@
       <c r="B30" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
       <c r="E30" s="1" t="s">
         <v>31</v>
+      </c>
+      <c r="F30" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
       <c r="E31" s="1" t="s">
         <v>33</v>
+      </c>
+      <c r="F31" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="s">
         <v>34</v>
       </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
       <c r="E32" s="1" t="s">
         <v>35</v>
+      </c>
+      <c r="F32" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="s">
         <v>36</v>
       </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
       <c r="E33" s="1" t="s">
         <v>37</v>
+      </c>
+      <c r="F33" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34" s="3" t="s">
         <v>38</v>
       </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
       <c r="E34" s="1" t="s">
         <v>39</v>
+      </c>
+      <c r="F34" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B35" s="3" t="s">
         <v>40</v>
       </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
       <c r="E35" s="1" t="s">
         <v>41</v>
+      </c>
+      <c r="F35" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">

</xml_diff>